<commit_message>
Updated CHiLO Producer to ver. 2
- For details, see Release Note
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chilo-producer\chiloPro\template-series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16635" windowHeight="7785"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21795" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="series-information" sheetId="37" r:id="rId1"/>
@@ -254,8 +254,380 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
+    <t>表紙画像
+―――――――――――――
+表紙画像のファイル名（表紙画像が無い場合は空白にしてください）</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウシ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>identifier</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>revised</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>改訂版発行日</t>
+    <rPh sb="0" eb="3">
+      <t>カイテイバン</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ハッコウビ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vol-1</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>video-id</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>書籍の言語</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>* 必須</t>
+    <rPh sb="2" eb="4">
+      <t>ヒッス</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>* 必須
+* 「Copyright」ページに挿入されます。記載しない場合は、項目自体が表示されません。</t>
+    <rPh sb="2" eb="4">
+      <t>ヒッス</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ソウニュウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CHiLO Bookのシリーズ名</t>
+    <rPh sb="15" eb="16">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>初版発行日</t>
+    <rPh sb="0" eb="2">
+      <t>ショハン</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>ハッコウビ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>* 「はじめにお読みください」セクションの「シリーズの紹介」ページに挿入されます。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>* 「シリーズの紹介」ページのシリーズの紹介文の下に挿入されます。</t>
+    <rPh sb="20" eb="22">
+      <t>ショウカイ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ブン</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>シタ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>* 各セクションの内表紙画像として使用されます。</t>
+    <rPh sb="2" eb="3">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒョウシ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>著者名</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>section（必須）</t>
+    <rPh sb="8" eb="10">
+      <t>ヒッス</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>topic</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>structure-books.xlsxのバージョン</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>（必須）巻数
+──────
+「vol-数字」
+の形式で順に記載します。</t>
+    <rPh sb="1" eb="3">
+      <t>ヒッス</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>サッスウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ケイシキ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ジュン</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>series-name</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CHiLO BookのユニークID。
+──────────────────
+content.opfに設定されます。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>各CHiLO Bookの概要
+────────────
+「はじめにお読みください」セクションの「ブック概要」に挿入されます。</t>
+    <rPh sb="0" eb="1">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ソウニュウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>セクションタイトル
+────────</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Javascriptのファイル名
+─────
+ページに組み込むJavascriptのファイル名を記入してください。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ページタイプ
+──────
+ページのタイプ
+document
+…ビデオ解説ページ
+test
+…クイズページ
+小文字で入力してください。</t>
+    <rPh sb="35" eb="37">
+      <t>カイセツ</t>
+    </rPh>
+    <rPh sb="54" eb="57">
+      <t>コモジ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>SNSのURL
+────────────
+Facebook、Twitter、Moodleフォーラムなど、任意のSNSを学習コミュニティとして指定できます。
+記載しない場合は、コミュニティアイコンが表示されません。</t>
+    <rPh sb="52" eb="54">
+      <t>ニンイ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>* 必須　authors.xlsxのシート名と一致させてください。</t>
+    <rPh sb="2" eb="4">
+      <t>ヒッス</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>・ シリーズに関する情報を記載するシートです。
+・ 色のついているセルは必須項目です。
+・ 変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。</t>
+  </si>
+  <si>
+    <t>・ シリーズの各ブックに関する情報を記載するシートです。
+・ 色のついているセルは必須項目です。
+・ 制作するブックの冊数分だけ、行を挿入して必要事項を記載ください。
+・ 変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。</t>
+  </si>
+  <si>
+    <t>コミュニティの表示
+──────────
+ページのコミュニティリンクボタンの表示非表示を指定できます。リンクボタンの表示する場合は、「TRUE」とします。book-listシートのcommunity-url項目を記載した場合のみ有効です。</t>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>解説ビデオサムネイルのファイル名
+────────────
+page-type項目を「document」とした場合のみ有効です。</t>
+    <rPh sb="0" eb="2">
+      <t>カイセツ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>解説文のファイル名
+─────
+page-type項目を「document」とした場合のみ有効です。</t>
+    <rPh sb="0" eb="2">
+      <t>カイセツ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t xml:space="preserve">・ ブックの解説ページと確認テストページに関するシートです。
+・ 色のついているセルは必須項目です。
+・ page-typeを指定して、行を追加するとCHiLO Bookのページが追加されます。
+・ ブックの数だけ書籍構成シートをコピーして、1冊のブックにつき1シート作成します。
+・ シート名は、book-listの「vol」の列と一致させてください。
+・変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。
+</t>
+  </si>
+  <si>
+    <t>トピックタイトル
+───────
+page-type項目を「document」とした場合のみ有効です。「test」とした場合は記載する必要がありません。</t>
+    <rPh sb="63" eb="65">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CCのライセンス
+────────
+CCライセンスでない場合は記載する必要がありません。</t>
+    <rPh sb="28" eb="30">
+      <t>ナイバアイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CHiLO Bookのタイトル
+────────────
+実際の書先タイトルは、
+「series-name 第n章 book-title」
+となります。series-nameは、series-informationシートのseries-name項目です。
+例）はじめての情報ネットワークI 第1章インターネットの歴史とビットの復習
+この書籍タイトルは、content.opfに設定されるほか、「Copyright」ページに挿入されます。</t>
+    <rPh sb="10" eb="11">
+      <t>ホンンオ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>あくまでも、structure-books.xlsxファイルの管理用であり、CHiLO Bookの書き出しには使われていません。ご自由に設定ください。</t>
+  </si>
+  <si>
+    <t>* 必須　ja, enなど、言語をRFC 5646形式で記載します。</t>
+    <rPh sb="2" eb="4">
+      <t>ヒッス</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ケイシキ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
     <r>
-      <t>c</t>
+      <t>b</t>
     </r>
     <r>
       <rPr>
@@ -266,196 +638,15 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>over</t>
+      <t>ook-cover</t>
     </r>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>表紙画像
-―――――――――――――
-表紙画像のファイル名（表紙画像が無い場合は空白にしてください）</t>
-    <rPh sb="0" eb="2">
-      <t>ヒョウシ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>identifier</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>revised</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>改訂版発行日</t>
-    <rPh sb="0" eb="3">
-      <t>カイテイバン</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>ハッコウビ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>vol-1</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>community</t>
-  </si>
-  <si>
-    <t>video-id</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>書籍の言語</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>* 必須</t>
-    <rPh sb="2" eb="4">
-      <t>ヒッス</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>* 必須
-* 「Copyright」ページに挿入されます。記載しない場合は、項目自体が表示されません。</t>
-    <rPh sb="2" eb="4">
-      <t>ヒッス</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ソウニュウ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>CHiLO Bookのシリーズ名</t>
-    <rPh sb="15" eb="16">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>初版発行日</t>
-    <rPh sb="0" eb="2">
-      <t>ショハン</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>ハッコウビ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>* 「はじめにお読みください」セクションの「シリーズの紹介」ページに挿入されます。</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>* 「シリーズの紹介」ページのシリーズの紹介文の下に挿入されます。</t>
-    <rPh sb="20" eb="22">
-      <t>ショウカイ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>ブン</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>シタ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>* 各セクションの内表紙画像として使用されます。</t>
-    <rPh sb="2" eb="3">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ウチ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒョウシ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ガゾウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>シヨウ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>著者名</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>section（必須）</t>
-    <rPh sb="8" eb="10">
-      <t>ヒッス</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>topic</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>structure-books.xlsxのバージョン</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>（必須）巻数
-──────
-「vol-数字」
-の形式で順に記載します。</t>
-    <rPh sb="1" eb="3">
-      <t>ヒッス</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>カン</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>サッスウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ケイシキ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ジュン</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>キサイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>series-name</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>各CHiLO Bookの概要
-────────────
-「はじめにお読みください」セクションの「ブック概要」に挿入されます。</t>
-    <rPh sb="0" eb="1">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ソウニュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>セクションタイトル
-────────</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>ページのメインコンテンツ
 ────────────
 page-typeによって指定するメインコンテンツが違います。
-document…解説ビデオのファイル名
+document…解説ビデオまたは音声のファイル名
 test…MoodleクイズのURL</t>
     <rPh sb="39" eb="41">
       <t>シテイ</t>
@@ -466,200 +657,12 @@
     <rPh sb="67" eb="69">
       <t>カイセツ</t>
     </rPh>
-    <rPh sb="77" eb="78">
+    <rPh sb="75" eb="77">
+      <t>オンセイ</t>
+    </rPh>
+    <rPh sb="82" eb="83">
       <t>メイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Javascriptのファイル名
-─────
-ページに組み込むJavascriptのファイル名を記入してください。</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ページタイプ
-──────
-ページのタイプ
-document
-…ビデオ解説ページ
-test
-…クイズページ
-小文字で入力してください。</t>
-    <rPh sb="35" eb="37">
-      <t>カイセツ</t>
-    </rPh>
-    <rPh sb="54" eb="57">
-      <t>コモジ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>SNSのURL
-────────────
-Facebook、Twitter、Moodleフォーラムなど、任意のSNSを学習コミュニティとして指定できます。
-記載しない場合は、コミュニティアイコンが表示されません。</t>
-    <rPh sb="52" eb="54">
-      <t>ニンイ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>* 必須　authors.xlsxのシート名と一致させてください。</t>
-    <rPh sb="2" eb="4">
-      <t>ヒッス</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>・ シリーズに関する情報を記載するシートです。
-・ 色のついているセルは必須項目です。
-・ 変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。</t>
-  </si>
-  <si>
-    <t>・ シリーズの各ブックに関する情報を記載するシートです。
-・ 色のついているセルは必須項目です。
-・ 制作するブックの冊数分だけ、行を挿入して必要事項を記載ください。
-・ 変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。</t>
-  </si>
-  <si>
-    <t>コミュニティの表示
-──────────
-ページのコミュニティリンクボタンの表示非表示を指定できます。リンクボタンの表示する場合は、「TRUE」とします。book-listシートのcommunity-url項目を記載した場合のみ有効です。</t>
-    <rPh sb="7" eb="9">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>解説ビデオサムネイルのファイル名
-────────────
-page-type項目を「document」とした場合のみ有効です。</t>
-    <rPh sb="0" eb="2">
-      <t>カイセツ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>解説文のファイル名
-─────
-page-type項目を「document」とした場合のみ有効です。</t>
-    <rPh sb="0" eb="2">
-      <t>カイセツ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t xml:space="preserve">・ ブックの解説ページと確認テストページに関するシートです。
-・ 色のついているセルは必須項目です。
-・ page-typeを指定して、行を追加するとCHiLO Bookのページが追加されます。
-・ ブックの数だけ書籍構成シートをコピーして、1冊のブックにつき1シート作成します。
-・ シート名は、book-listの「vol」の列と一致させてください。
-・変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。
-</t>
-  </si>
-  <si>
-    <t>トピックタイトル
-───────
-page-type項目を「document」とした場合のみ有効です。「test」とした場合は記載する必要がありません。</t>
-    <rPh sb="63" eb="65">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>CCのライセンス
-────────
-CCライセンスでない場合は記載する必要がありません。</t>
-    <rPh sb="28" eb="30">
-      <t>ナイバアイ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>CHiLO Bookのタイトル
-────────────
-実際の書先タイトルは、
-「series-name 第n章 book-title」
-となります。series-nameは、series-informationシートのseries-name項目です。
-例）はじめての情報ネットワークI 第1章インターネットの歴史とビットの復習
-この書籍タイトルは、content.opfに設定されるほか、「Copyright」ページに挿入されます。</t>
-    <rPh sb="10" eb="11">
-      <t>ホンンオ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>ショウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>あくまでも、structure-books.xlsxファイルの管理用であり、CHiLO Bookの書き出しには使われていません。ご自由に設定ください。</t>
-  </si>
-  <si>
-    <t>* 必須　ja, enなど、言語をRFC 5646形式で記載します。</t>
-    <rPh sb="2" eb="4">
-      <t>ヒッス</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ゲンゴ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ケイシキ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>キサイ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>（必須）CHiLO BookのユニークID。
-──────────────────
-content.opfに設定されます。</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1277,7 +1280,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1463,6 +1466,14 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1480,6 +1491,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1940,10 +1954,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1">
@@ -1952,10 +1966,10 @@
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1">
@@ -1964,10 +1978,10 @@
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
@@ -1978,8 +1992,8 @@
       <c r="C4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="59" t="s">
-        <v>51</v>
+      <c r="D4" s="62" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1">
@@ -1990,7 +2004,7 @@
       <c r="C5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="60"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
       <c r="A6" s="31" t="s">
@@ -1998,19 +2012,19 @@
       </c>
       <c r="B6" s="53"/>
       <c r="C6" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="60"/>
+        <v>52</v>
+      </c>
+      <c r="D6" s="63"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
       <c r="A8" s="31" t="s">
@@ -2020,18 +2034,18 @@
       <c r="C8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="61"/>
+      <c r="D8" s="64"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1">
-      <c r="A9" s="57" t="s">
-        <v>62</v>
+      <c r="A9" s="59" t="s">
+        <v>61</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="80.099999999999994" customHeight="1">
@@ -2043,7 +2057,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1">
@@ -2055,7 +2069,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1">
@@ -2067,7 +2081,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2078,26 +2092,26 @@
       <c r="D13" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
-      <c r="A15" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
+      <c r="A15" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="65"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="68"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2138,22 +2152,22 @@
       <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>41</v>
+      <c r="D1" s="61" t="s">
+        <v>80</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="48" customHeight="1" thickTop="1">
-      <c r="A2" s="54" t="s">
-        <v>46</v>
+      <c r="A2" s="56" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="49"/>
-      <c r="C2" s="56"/>
+      <c r="C2" s="58"/>
       <c r="D2" s="44"/>
       <c r="E2" s="54"/>
       <c r="F2" s="50"/>
@@ -2171,27 +2185,27 @@
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
-      <c r="E4" s="51"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" ht="253.5">
       <c r="A5" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2213,36 +2227,36 @@
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
+      <c r="B9" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
       <c r="F9" s="46"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
       <c r="F10" s="46"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="76"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
       <c r="F11" s="46"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="79"/>
       <c r="F12" s="46"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="77"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="79"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="82"/>
       <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:6">
@@ -2287,13 +2301,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>47</v>
+      <c r="D1" s="57" t="s">
+        <v>46</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>1</v>
@@ -2308,7 +2322,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>5</v>
@@ -2316,8 +2330,8 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="20.25" thickTop="1">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
       <c r="C2" s="11"/>
       <c r="D2" s="42"/>
       <c r="E2" s="11"/>
@@ -2329,8 +2343,8 @@
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="11"/>
       <c r="D3" s="42"/>
       <c r="E3" s="11"/>
@@ -2342,8 +2356,8 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="11"/>
       <c r="D4" s="42"/>
       <c r="E4" s="11"/>
@@ -2355,8 +2369,8 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="11"/>
       <c r="D5" s="42"/>
       <c r="E5" s="11"/>
@@ -2368,8 +2382,8 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="58"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="11"/>
       <c r="D6" s="42"/>
       <c r="E6" s="11"/>
@@ -2381,8 +2395,8 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="11"/>
       <c r="D7" s="42"/>
       <c r="E7" s="11"/>
@@ -2394,8 +2408,8 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="11"/>
       <c r="D8" s="42"/>
       <c r="E8" s="11"/>
@@ -2407,8 +2421,8 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="11"/>
       <c r="D9" s="42"/>
       <c r="E9" s="11"/>
@@ -2420,8 +2434,8 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="11"/>
       <c r="D10" s="42"/>
       <c r="E10" s="11"/>
@@ -2433,8 +2447,8 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="58"/>
-      <c r="B11" s="58"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="11"/>
       <c r="D11" s="42"/>
       <c r="E11" s="11"/>
@@ -2446,8 +2460,8 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="58"/>
-      <c r="B12" s="58"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="11"/>
       <c r="D12" s="42"/>
       <c r="E12" s="11"/>
@@ -2459,8 +2473,8 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="58"/>
-      <c r="B13" s="58"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="11"/>
       <c r="D13" s="42"/>
       <c r="E13" s="11"/>
@@ -2472,8 +2486,8 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="58"/>
-      <c r="B14" s="58"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="11"/>
       <c r="D14" s="42"/>
       <c r="E14" s="11"/>
@@ -2485,8 +2499,8 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="11"/>
       <c r="D15" s="42"/>
       <c r="E15" s="11"/>
@@ -2498,8 +2512,8 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="11"/>
       <c r="D16" s="42"/>
       <c r="E16" s="12"/>
@@ -2527,34 +2541,34 @@
     </row>
     <row r="18" spans="1:11" s="39" customFormat="1" ht="165" customHeight="1">
       <c r="A18" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="36" t="s">
         <v>64</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="G18" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="36" t="s">
-        <v>66</v>
       </c>
       <c r="I18" s="36" t="s">
         <v>40</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K18" s="38"/>
     </row>
@@ -2567,48 +2581,48 @@
       <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
-      <c r="B21" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="82"/>
+      <c r="B21" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="85"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="83"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="85"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="88"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="B23" s="83"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="85"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="88"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="85"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="88"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="B25" s="83"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="85"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="88"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="B26" s="83"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="85"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="88"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="88"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
Set inside cover for each CHiLO Book
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitsuhashi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>cover</t>
     <phoneticPr fontId="4"/>
@@ -172,10 +172,6 @@
   </si>
   <si>
     <t>language</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>creator</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -665,6 +661,177 @@
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uthor</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>published</t>
+  </si>
+  <si>
+    <t>revised</t>
+  </si>
+  <si>
+    <t>rights</t>
+  </si>
+  <si>
+    <r>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nside-cover</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>章ごとに変更するシリーズ情報
+────────────
+[series-information]の情報のうち、章ごとに変更したい箇所があればここに記入します。
+（[series-information]と同じ情報を使いたい場合は、空白のままにしてください）</t>
+    <rPh sb="0" eb="1">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>カショ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>キニュウ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>クウハク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>章ごとに変更する内表紙画像
+────────────
+[series-information]の内表紙画像を章ごとに変更したい箇所が荒れれば、画像を vol-n/imagesに保存し、ファイル名をここに記入します。
+（[series-information]と同じ内表紙を使いたい場合は、空白のままにしてください）</t>
+    <rPh sb="0" eb="1">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヒョウシ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ヒョウシ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>カショ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="96" eb="97">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>キニュウ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="132" eb="133">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ヒョウシ</t>
+    </rPh>
+    <rPh sb="136" eb="137">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="140" eb="142">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="144" eb="146">
+      <t>クウハク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
@@ -673,7 +840,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,8 +977,24 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -842,8 +1025,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1100,6 +1289,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1280,7 +1480,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1296,9 +1496,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1350,9 +1547,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1362,9 +1556,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1492,7 +1683,16 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1593,6 +1793,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1942,158 +2166,158 @@
     <col min="1" max="1" width="21.125" customWidth="1"/>
     <col min="2" max="2" width="55.625" customWidth="1"/>
     <col min="3" max="3" width="46.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="75.625" style="22" customWidth="1"/>
     <col min="5" max="5" width="48.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="29">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21" customHeight="1">
+      <c r="A2" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" customHeight="1">
+      <c r="A3" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1">
+      <c r="A4" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21" customHeight="1">
+      <c r="A5" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="63"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1">
+      <c r="A6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="50"/>
+      <c r="C6" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="63"/>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1">
+      <c r="A7" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="63"/>
+    </row>
+    <row r="8" spans="1:4" ht="21" customHeight="1">
+      <c r="A8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="64"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1">
+      <c r="A9" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="80.099999999999994" customHeight="1">
+      <c r="A10" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1">
+      <c r="A11" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1">
+      <c r="A12" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="32">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="21" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1">
-      <c r="A3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1">
-      <c r="A4" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1">
-      <c r="A5" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="63"/>
-    </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1">
-      <c r="A6" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="63"/>
-    </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1">
-      <c r="A7" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="63"/>
-    </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1">
-      <c r="A8" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="64"/>
-    </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1">
-      <c r="A9" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="80.099999999999994" customHeight="1">
-      <c r="A10" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1">
-      <c r="A11" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1">
-      <c r="A12" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
@@ -2114,6 +2338,7 @@
       <c r="C18" s="73"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="D4:D8"/>
     <mergeCell ref="A15:C18"/>
@@ -2127,7 +2352,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2139,133 +2364,209 @@
     <col min="4" max="4" width="32.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="43.125" style="2" customWidth="1"/>
     <col min="6" max="6" width="37.875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="2"/>
+    <col min="7" max="7" width="8.375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.75" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="61" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="61" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42" style="61" customWidth="1"/>
+    <col min="16" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:15" ht="20.25" thickBot="1">
+      <c r="A1" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="92" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1" thickTop="1">
-      <c r="A2" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="50"/>
-    </row>
-    <row r="3" spans="1:6" ht="48" customHeight="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="4" spans="1:6" ht="48" customHeight="1">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="52"/>
-    </row>
-    <row r="5" spans="1:6" ht="253.5">
-      <c r="A5" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="G1" s="95" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="95" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="95" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="95" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="48" customHeight="1" thickTop="1">
+      <c r="A2" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+    </row>
+    <row r="3" spans="1:15" ht="48" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+    </row>
+    <row r="4" spans="1:15" ht="48" customHeight="1">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+    </row>
+    <row r="5" spans="1:15" ht="253.5">
+      <c r="A5" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="F6" s="40"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A9" s="6"/>
+      <c r="D5" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="99" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="F6" s="37"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A9" s="5"/>
       <c r="B9" s="74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="75"/>
       <c r="D9" s="76"/>
-      <c r="F9" s="46"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="6"/>
+      <c r="F9" s="43"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="5"/>
       <c r="B10" s="77"/>
       <c r="C10" s="78"/>
       <c r="D10" s="79"/>
-      <c r="F10" s="46"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="43"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="B11" s="77"/>
       <c r="C11" s="78"/>
       <c r="D11" s="79"/>
-      <c r="F11" s="46"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="43"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="B12" s="77"/>
       <c r="C12" s="78"/>
       <c r="D12" s="79"/>
-      <c r="F12" s="46"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="43"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="B13" s="80"/>
       <c r="C13" s="81"/>
       <c r="D13" s="82"/>
-      <c r="F13" s="46"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="F14" s="47"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="F14" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="1">
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="2">
     <mergeCell ref="B9:D13"/>
+    <mergeCell ref="G5:N5"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2282,307 +2583,307 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="19" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="25" style="9" customWidth="1"/>
-    <col min="5" max="5" width="40.625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="30.625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="25" style="8" customWidth="1"/>
-    <col min="9" max="9" width="37.5" style="8" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="21.625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25" style="8" customWidth="1"/>
+    <col min="5" max="5" width="40.625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="30.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="25" style="7" customWidth="1"/>
+    <col min="9" max="9" width="37.5" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.875" style="7" customWidth="1"/>
     <col min="11" max="11" width="8.875" style="4"/>
-    <col min="12" max="16384" width="8.875" style="8"/>
+    <col min="12" max="16384" width="8.875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" ht="20.25" thickBot="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="20.25" thickTop="1">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="10"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="10"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="10"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="10"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="10"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="60"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="10"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="10"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="60"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="10"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="10"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="10"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="10"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="10"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="10"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="10"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="1:11" s="19" customFormat="1">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" s="18" customFormat="1">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="39" customFormat="1" ht="165" customHeight="1">
-      <c r="A18" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="36" t="s">
+    <row r="18" spans="1:11" s="36" customFormat="1" ht="165" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="I18" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="K18" s="38"/>
-    </row>
-    <row r="19" spans="1:11" s="16" customFormat="1">
-      <c r="D19" s="17"/>
-      <c r="K19" s="18"/>
-    </row>
-    <row r="20" spans="1:11" s="16" customFormat="1">
-      <c r="D20" s="17"/>
-      <c r="K20" s="18"/>
+      <c r="K18" s="35"/>
+    </row>
+    <row r="19" spans="1:11" s="15" customFormat="1">
+      <c r="D19" s="16"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="1:11" s="15" customFormat="1">
+      <c r="D20" s="16"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="B21" s="83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84"/>
@@ -2625,7 +2926,7 @@
       <c r="E27" s="91"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="B21:E27"/>
   </mergeCells>
@@ -2674,68 +2975,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickTop="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
Added begin and end column on the vol-n sheet
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitsuhashi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>cover</t>
     <phoneticPr fontId="4"/>
@@ -829,6 +829,74 @@
     </rPh>
     <rPh sb="144" eb="146">
       <t>クウハク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>begin</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>end</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>動画分割の開始位置
+─────
+動画をページ毎に分割する場合の、開始位置を秒数で指定します。</t>
+    <rPh sb="0" eb="2">
+      <t>ドウガ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ブンカツ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ドウガ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ゴト</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ブンカツ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ビョウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>スウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>動画分割の終了位置
+─────
+動画をページ分割する場合の、終了位置を秒数で指定します。</t>
+    <rPh sb="0" eb="2">
+      <t>ドウガ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>シュウリョウ</t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -1695,6 +1763,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1758,6 +1844,12 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1793,30 +1885,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -2216,7 +2284,7 @@
       <c r="C4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="68" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2228,7 +2296,7 @@
       <c r="C5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="63"/>
+      <c r="D5" s="69"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
       <c r="A6" s="28" t="s">
@@ -2238,7 +2306,7 @@
       <c r="C6" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="69"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1">
       <c r="A7" s="28" t="s">
@@ -2248,7 +2316,7 @@
       <c r="C7" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="63"/>
+      <c r="D7" s="69"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
       <c r="A8" s="28" t="s">
@@ -2258,7 +2326,7 @@
       <c r="C8" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="64"/>
+      <c r="D8" s="70"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1">
       <c r="A9" s="56" t="s">
@@ -2316,26 +2384,26 @@
       <c r="D13" s="24"/>
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="73"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="68"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="70"/>
+      <c r="A16" s="74"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="76"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="71"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="73"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="79"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2376,49 +2444,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.25" thickBot="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="J1" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="95" t="s">
+      <c r="L1" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="95" t="s">
+      <c r="M1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="N1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="95" t="s">
+      <c r="O1" s="65" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2476,35 +2544,35 @@
       <c r="O4" s="58"/>
     </row>
     <row r="5" spans="1:15" ht="253.5">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="96" t="s">
+      <c r="E5" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="96" t="s">
+      <c r="F5" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="99" t="s">
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="67" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2527,36 +2595,36 @@
     </row>
     <row r="9" spans="1:15" ht="14.25" customHeight="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="82"/>
       <c r="F9" s="43"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="79"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="85"/>
       <c r="F10" s="43"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="B11" s="77"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="79"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="85"/>
       <c r="F11" s="43"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="79"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="85"/>
       <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="82"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="88"/>
       <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:15">
@@ -2577,7 +2645,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2591,13 +2659,14 @@
     <col min="6" max="6" width="30.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.125" style="7" customWidth="1"/>
     <col min="8" max="8" width="25" style="7" customWidth="1"/>
-    <col min="9" max="9" width="37.5" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5" style="7" customWidth="1"/>
     <col min="10" max="10" width="17.875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="8.875" style="4"/>
-    <col min="12" max="16384" width="8.875" style="7"/>
+    <col min="11" max="12" width="37.5" style="7" customWidth="1"/>
+    <col min="13" max="13" width="8.875" style="4"/>
+    <col min="14" max="16384" width="8.875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:13" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
@@ -2628,9 +2697,15 @@
       <c r="J1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="20.25" thickTop="1">
+      <c r="K1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.25" thickTop="1">
       <c r="A2" s="57"/>
       <c r="B2" s="57"/>
       <c r="C2" s="10"/>
@@ -2641,9 +2716,11 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="57"/>
       <c r="B3" s="57"/>
       <c r="C3" s="10"/>
@@ -2654,9 +2731,11 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="57"/>
       <c r="B4" s="57"/>
       <c r="C4" s="10"/>
@@ -2667,9 +2746,11 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="57"/>
       <c r="B5" s="57"/>
       <c r="C5" s="10"/>
@@ -2680,9 +2761,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="57"/>
       <c r="B6" s="57"/>
       <c r="C6" s="10"/>
@@ -2693,9 +2776,11 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="57"/>
       <c r="B7" s="57"/>
       <c r="C7" s="10"/>
@@ -2706,9 +2791,11 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="57"/>
       <c r="B8" s="57"/>
       <c r="C8" s="10"/>
@@ -2719,9 +2806,11 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="57"/>
       <c r="B9" s="57"/>
       <c r="C9" s="10"/>
@@ -2732,9 +2821,11 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="57"/>
       <c r="B10" s="57"/>
       <c r="C10" s="10"/>
@@ -2745,9 +2836,11 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="57"/>
       <c r="B11" s="57"/>
       <c r="C11" s="10"/>
@@ -2758,9 +2851,11 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="57"/>
       <c r="B12" s="57"/>
       <c r="C12" s="10"/>
@@ -2771,9 +2866,11 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="57"/>
       <c r="B13" s="57"/>
       <c r="C13" s="10"/>
@@ -2784,9 +2881,11 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="57"/>
       <c r="B14" s="57"/>
       <c r="C14" s="10"/>
@@ -2797,9 +2896,11 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="57"/>
       <c r="B15" s="57"/>
       <c r="C15" s="10"/>
@@ -2810,9 +2911,11 @@
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="57"/>
       <c r="B16" s="57"/>
       <c r="C16" s="10"/>
@@ -2823,9 +2926,11 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" s="18" customFormat="1">
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" s="18" customFormat="1">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
@@ -2836,11 +2941,13 @@
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="36" customFormat="1" ht="165" customHeight="1">
+    <row r="18" spans="1:13" s="36" customFormat="1" ht="165" customHeight="1">
       <c r="A18" s="33" t="s">
         <v>65</v>
       </c>
@@ -2871,59 +2978,65 @@
       <c r="J18" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="35"/>
-    </row>
-    <row r="19" spans="1:11" s="15" customFormat="1">
+      <c r="K18" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="L18" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="M18" s="35"/>
+    </row>
+    <row r="19" spans="1:13" s="15" customFormat="1">
       <c r="D19" s="16"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" s="15" customFormat="1">
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" s="15" customFormat="1">
       <c r="D20" s="16"/>
-      <c r="K20" s="17"/>
-    </row>
-    <row r="21" spans="1:11" ht="14.25" customHeight="1">
-      <c r="B21" s="83" t="s">
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" ht="14.25" customHeight="1">
+      <c r="B21" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="85"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="B22" s="86"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="88"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="88"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="B24" s="86"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="88"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="B25" s="86"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="88"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="B26" s="86"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="88"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="93"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="B22" s="94"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="B24" s="94"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="96"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="B25" s="94"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="96"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="B26" s="94"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="B27" s="97"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="99"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
closed #29 Allow editing series-information cell in book-list
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chilo-producer\chiloPro\template-series\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21795" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21795" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="series-information" sheetId="37" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
   <si>
     <t>cover</t>
     <phoneticPr fontId="4"/>
@@ -682,16 +682,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>publisher</t>
-  </si>
-  <si>
-    <t>editor</t>
-  </si>
-  <si>
     <t>published</t>
-  </si>
-  <si>
-    <t>revised</t>
   </si>
   <si>
     <t>rights</t>
@@ -898,6 +889,22 @@
     <rPh sb="30" eb="32">
       <t>シュウリョウ</t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>version</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>revised</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>publisher</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>editor</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1548,7 +1555,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1564,12 +1571,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <alignment vertical="center"/>
@@ -1673,9 +1674,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="37" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1687,78 +1685,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="37" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1815,33 +1757,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1885,6 +1800,93 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="37" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -2227,183 +2229,183 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="21.125" customWidth="1"/>
     <col min="2" max="2" width="55.625" customWidth="1"/>
     <col min="3" max="3" width="46.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="75.625" style="20" customWidth="1"/>
     <col min="5" max="5" width="48.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="29">
+      <c r="B1" s="27">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="50" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="27" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="69"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="70"/>
+      <c r="D8" s="52"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="80.099999999999994" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="24" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="24" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="73"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="74"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="76"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="74"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="76"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="77"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="61"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2422,7 +2424,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="19.5"/>
   <cols>
@@ -2432,206 +2434,281 @@
     <col min="4" max="4" width="32.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="43.125" style="2" customWidth="1"/>
     <col min="6" max="6" width="37.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.375" style="61" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.125" style="61" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.75" style="61" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="61" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.625" style="61" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5" style="61" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.625" style="61" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42" style="61" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.75" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" style="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.625" style="43" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42" style="43" customWidth="1"/>
     <col min="16" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" thickBot="1">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:15" s="81" customFormat="1" ht="20.25" thickBot="1">
+      <c r="A1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="65" t="s">
+      <c r="G1" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="I1" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="J1" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="65" t="s">
+      <c r="M1" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="O1" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="65" t="s">
+    </row>
+    <row r="2" spans="1:15" s="81" customFormat="1" ht="48" customHeight="1" thickTop="1">
+      <c r="A2" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+    </row>
+    <row r="3" spans="1:15" s="81" customFormat="1" ht="48" customHeight="1">
+      <c r="A3" s="82"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+    </row>
+    <row r="4" spans="1:15" s="81" customFormat="1" ht="48" customHeight="1">
+      <c r="A4" s="85"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+    </row>
+    <row r="5" spans="1:15" s="81" customFormat="1" ht="253.5">
+      <c r="A5" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="65" t="s">
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="48" customHeight="1" thickTop="1">
-      <c r="A2" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-    </row>
-    <row r="3" spans="1:15" ht="48" customHeight="1">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-    </row>
-    <row r="4" spans="1:15" ht="48" customHeight="1">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-    </row>
-    <row r="5" spans="1:15" ht="253.5">
-      <c r="A5" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="89" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="F6" s="37"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="80" t="s">
+    </row>
+    <row r="6" spans="1:15" s="81" customFormat="1">
+      <c r="A6" s="88"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+    </row>
+    <row r="7" spans="1:15" s="81" customFormat="1">
+      <c r="F7" s="90"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+    </row>
+    <row r="8" spans="1:15" s="81" customFormat="1">
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="89"/>
+      <c r="O8" s="89"/>
+    </row>
+    <row r="9" spans="1:15" s="81" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A9" s="91"/>
+      <c r="B9" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
-      <c r="F9" s="43"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="85"/>
-      <c r="F10" s="43"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="85"/>
-      <c r="F11" s="43"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="85"/>
-      <c r="F12" s="43"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="B13" s="86"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="88"/>
-      <c r="F13" s="43"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+    </row>
+    <row r="10" spans="1:15" s="81" customFormat="1">
+      <c r="A10" s="91"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="98"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+    </row>
+    <row r="11" spans="1:15" s="81" customFormat="1">
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="98"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+    </row>
+    <row r="12" spans="1:15" s="81" customFormat="1">
+      <c r="B12" s="96"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="98"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+    </row>
+    <row r="13" spans="1:15" s="81" customFormat="1">
+      <c r="B13" s="99"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="101"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="F14" s="44"/>
+      <c r="F14" s="38"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <protectedRanges>
+    <protectedRange sqref="A2:XFD4" name="範囲1"/>
+  </protectedRanges>
   <mergeCells count="2">
     <mergeCell ref="B9:D13"/>
     <mergeCell ref="G5:N5"/>
@@ -2651,392 +2728,392 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="19" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="25" style="8" customWidth="1"/>
-    <col min="5" max="5" width="40.625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="30.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="25" style="7" customWidth="1"/>
-    <col min="9" max="9" width="37.5" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.875" style="7" customWidth="1"/>
-    <col min="11" max="12" width="37.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="21.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25" style="6" customWidth="1"/>
+    <col min="5" max="5" width="40.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="30.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25" style="5" customWidth="1"/>
+    <col min="9" max="9" width="37.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.875" style="5" customWidth="1"/>
+    <col min="11" max="12" width="37.5" style="5" customWidth="1"/>
     <col min="13" max="13" width="8.875" style="4"/>
-    <col min="14" max="16384" width="8.875" style="7"/>
+    <col min="14" max="16384" width="8.875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" ht="20.25" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>92</v>
+      <c r="K1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="20.25" thickTop="1">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="9"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="9"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="9"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="9"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="9"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="9"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="57"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="9"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="57"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="9"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="57"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="9"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="57"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="9"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="9"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="9"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="9"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="9"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" s="18" customFormat="1">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" s="16" customFormat="1">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="36" customFormat="1" ht="165" customHeight="1">
-      <c r="A18" s="33" t="s">
+    <row r="18" spans="1:13" s="34" customFormat="1" ht="165" customHeight="1">
+      <c r="A18" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="J18" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="L18" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="M18" s="35"/>
-    </row>
-    <row r="19" spans="1:13" s="15" customFormat="1">
-      <c r="D19" s="16"/>
-      <c r="M19" s="17"/>
-    </row>
-    <row r="20" spans="1:13" s="15" customFormat="1">
-      <c r="D20" s="16"/>
-      <c r="M20" s="17"/>
+      <c r="K18" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="M18" s="33"/>
+    </row>
+    <row r="19" spans="1:13" s="13" customFormat="1">
+      <c r="D19" s="14"/>
+      <c r="M19" s="15"/>
+    </row>
+    <row r="20" spans="1:13" s="13" customFormat="1">
+      <c r="D20" s="14"/>
+      <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="93"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="96"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="69"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="B23" s="94"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="96"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="B24" s="94"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="96"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="69"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="B25" s="94"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="96"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="B26" s="94"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="96"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="69"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="B27" s="97"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="99"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -3088,68 +3165,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
Set the default inside cover
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chilo-producer\chiloPro\template-series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>main</t>
   </si>
@@ -932,6 +932,10 @@
     <rPh sb="56" eb="57">
       <t>ショウ</t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>chilo_inside_cover.png</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -2397,7 +2401,9 @@
       <c r="A12" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="27" t="s">
+        <v>96</v>
+      </c>
       <c r="C12" s="25" t="s">
         <v>35</v>
       </c>
@@ -2451,7 +2457,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="19.5"/>
   <cols>

</xml_diff>

<commit_message>
closed #41 Reset the [book-list] sheet Lock Cells to Unlock Cells
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -1138,7 +1138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1395,17 +1395,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1751,172 +1740,187 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="37" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2317,7 +2321,7 @@
       <c r="C4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="55" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2329,7 +2333,7 @@
       <c r="C5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="71"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
       <c r="A6" s="26" t="s">
@@ -2339,7 +2343,7 @@
       <c r="C6" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="71"/>
+      <c r="D6" s="56"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1">
       <c r="A7" s="26" t="s">
@@ -2349,7 +2353,7 @@
       <c r="C7" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="56"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
       <c r="A8" s="26" t="s">
@@ -2359,7 +2363,7 @@
       <c r="C8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="72"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1">
       <c r="A9" s="41" t="s">
@@ -2419,26 +2423,26 @@
       <c r="D13" s="22"/>
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="75"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="76"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="63"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="79"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2457,9 +2461,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="19.5"/>
   <cols>
@@ -2480,7 +2482,7 @@
     <col min="16" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="58" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:15" s="49" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="44" t="s">
         <v>6</v>
       </c>
@@ -2527,60 +2529,60 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="58" customFormat="1" ht="48" customHeight="1" thickTop="1">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:15" s="49" customFormat="1" ht="48" customHeight="1" thickTop="1">
+      <c r="A2" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-    </row>
-    <row r="3" spans="1:15" s="58" customFormat="1" ht="48" customHeight="1">
-      <c r="A3" s="59"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-    </row>
-    <row r="4" spans="1:15" s="58" customFormat="1" ht="48" customHeight="1">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-    </row>
-    <row r="5" spans="1:15" s="58" customFormat="1" ht="253.5">
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+    </row>
+    <row r="3" spans="1:15" s="49" customFormat="1" ht="48" customHeight="1">
+      <c r="A3" s="95"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+    </row>
+    <row r="4" spans="1:15" s="49" customFormat="1" ht="48" customHeight="1">
+      <c r="A4" s="98"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+    </row>
+    <row r="5" spans="1:15" s="49" customFormat="1" ht="253.5">
       <c r="A5" s="48" t="s">
         <v>56</v>
       </c>
@@ -2599,142 +2601,142 @@
       <c r="F5" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="G5" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="49" t="s">
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="86" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="58" customFormat="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-    </row>
-    <row r="7" spans="1:15" s="58" customFormat="1">
-      <c r="F7" s="67"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-    </row>
-    <row r="8" spans="1:15" s="58" customFormat="1">
-      <c r="A8" s="68"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-    </row>
-    <row r="9" spans="1:15" s="58" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A9" s="68"/>
-      <c r="B9" s="82" t="s">
+    <row r="6" spans="1:15" s="49" customFormat="1">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+    </row>
+    <row r="7" spans="1:15" s="49" customFormat="1">
+      <c r="F7" s="52"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+    </row>
+    <row r="8" spans="1:15" s="49" customFormat="1">
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+    </row>
+    <row r="9" spans="1:15" s="49" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A9" s="53"/>
+      <c r="B9" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="66"/>
-    </row>
-    <row r="10" spans="1:15" s="58" customFormat="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="87"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-    </row>
-    <row r="11" spans="1:15" s="58" customFormat="1">
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="87"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-    </row>
-    <row r="12" spans="1:15" s="58" customFormat="1">
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="87"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-    </row>
-    <row r="13" spans="1:15" s="58" customFormat="1">
-      <c r="B13" s="88"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="90"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="66"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+    </row>
+    <row r="10" spans="1:15" s="49" customFormat="1">
+      <c r="A10" s="53"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+    </row>
+    <row r="11" spans="1:15" s="49" customFormat="1">
+      <c r="B11" s="70"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+    </row>
+    <row r="12" spans="1:15" s="49" customFormat="1">
+      <c r="B12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="72"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+    </row>
+    <row r="13" spans="1:15" s="49" customFormat="1">
+      <c r="B13" s="73"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="75"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
     </row>
     <row r="14" spans="1:15">
       <c r="F14" s="38"/>
@@ -3107,48 +3109,48 @@
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B21" s="93" t="s">
+      <c r="B21" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="95"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="78"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="B22" s="96"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="98"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="B23" s="96"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="98"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="81"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="B24" s="96"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="98"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="81"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="B25" s="96"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="98"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="81"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="B26" s="96"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="98"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="81"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="B27" s="99"/>
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="101"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="84"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
closed # 42 Disable worksheet protection
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -468,17 +468,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>・ シリーズに関する情報を記載するシートです。
-・ 色のついているセルは必須項目です。
-・ 変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。</t>
-  </si>
-  <si>
-    <t>・ シリーズの各ブックに関する情報を記載するシートです。
-・ 色のついているセルは必須項目です。
-・ 制作するブックの冊数分だけ、行を挿入して必要事項を記載ください。
-・ 変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。</t>
-  </si>
-  <si>
     <t>コミュニティの表示
 ──────────
 ページのコミュニティリンクボタンの表示非表示を指定できます。リンクボタンの表示する場合は、「TRUE」とします。book-listシートのcommunity-url項目を記載した場合のみ有効です。</t>
@@ -522,15 +511,6 @@
       <t>メイ</t>
     </rPh>
     <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t xml:space="preserve">・ ブックの解説ページと確認テストページに関するシートです。
-・ 色のついているセルは必須項目です。
-・ page-typeを指定して、行を追加するとCHiLO Bookのページが追加されます。
-・ ブックの数だけ書籍構成シートをコピーして、1冊のブックにつき1シート作成します。
-・ シート名は、book-listの「vol」の列と一致させてください。
-・変更してはいけないセルに保護がかかっています。シートの保護解除のパスワードはつけていません。
-</t>
   </si>
   <si>
     <t>トピックタイトル
@@ -936,6 +916,25 @@
   </si>
   <si>
     <t>chilo_inside_cover.png</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>・ シリーズに関する情報を記載するシートです。
+・ 色のついているセルは必須項目です。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>・ シリーズの各ブックに関する情報を記載するシートです。
+・ 色のついているセルは必須項目です。
+・ 制作するブックの冊数分だけ、行を挿入して必要事項を記載ください。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>・ ブックの解説ページと確認テストページに関するシートです。
+・ 色のついているセルは必須項目です。
+・ page-typeを指定して、行を追加するとCHiLO Bookのページが追加されます。
+・ ブックの数だけ書籍構成シートをコピーして、1冊のブックにつき1シート作成します。
+・ シート名は、book-listの「vol」の列と一致させてください。</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1758,6 +1757,69 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="37" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1797,29 +1859,8 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1857,71 +1898,29 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="37" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -2262,7 +2261,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2286,7 +2285,7 @@
         <v>55</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1">
@@ -2298,12 +2297,12 @@
         <v>45</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1">
       <c r="A3" s="41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="25" t="s">
@@ -2321,7 +2320,7 @@
       <c r="C4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="71" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2333,7 +2332,7 @@
       <c r="C5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="72"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
       <c r="A6" s="26" t="s">
@@ -2341,9 +2340,9 @@
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="56"/>
+        <v>89</v>
+      </c>
+      <c r="D6" s="72"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1">
       <c r="A7" s="26" t="s">
@@ -2351,9 +2350,9 @@
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="56"/>
+        <v>90</v>
+      </c>
+      <c r="D7" s="72"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
       <c r="A8" s="26" t="s">
@@ -2363,7 +2362,7 @@
       <c r="C8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="57"/>
+      <c r="D8" s="73"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1">
       <c r="A9" s="41" t="s">
@@ -2403,10 +2402,10 @@
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1">
       <c r="A12" s="41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>35</v>
@@ -2423,32 +2422,26 @@
       <c r="D13" s="22"/>
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
-      <c r="A15" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="76"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="61"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="63"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="79"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="61"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="64"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="82"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="D4:D8"/>
-    <mergeCell ref="A15:C18"/>
+    <mergeCell ref="A15:C17"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2459,7 +2452,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2493,7 +2486,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E1" s="45" t="s">
         <v>40</v>
@@ -2502,92 +2495,92 @@
         <v>13</v>
       </c>
       <c r="G1" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="L1" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="O1" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="49" customFormat="1" ht="48" customHeight="1" thickTop="1">
-      <c r="A2" s="87" t="s">
+    </row>
+    <row r="2" spans="1:15" s="4" customFormat="1" ht="48" customHeight="1" thickTop="1">
+      <c r="A2" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-    </row>
-    <row r="3" spans="1:15" s="49" customFormat="1" ht="48" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-    </row>
-    <row r="4" spans="1:15" s="49" customFormat="1" ht="48" customHeight="1">
-      <c r="A4" s="98"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="48" customHeight="1">
+      <c r="A3" s="63"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+    </row>
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="48" customHeight="1">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
     </row>
     <row r="5" spans="1:15" s="49" customFormat="1" ht="253.5">
       <c r="A5" s="48" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>59</v>
@@ -2601,18 +2594,18 @@
       <c r="F5" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="86" t="s">
-        <v>83</v>
+      <c r="G5" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="55" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="49" customFormat="1">
@@ -2661,11 +2654,11 @@
     </row>
     <row r="9" spans="1:15" s="49" customFormat="1" ht="14.25" customHeight="1">
       <c r="A9" s="53"/>
-      <c r="B9" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="69"/>
+      <c r="B9" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="94"/>
+      <c r="D9" s="95"/>
       <c r="F9" s="54"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
@@ -2679,9 +2672,9 @@
     </row>
     <row r="10" spans="1:15" s="49" customFormat="1">
       <c r="A10" s="53"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="98"/>
       <c r="F10" s="54"/>
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
@@ -2694,9 +2687,9 @@
       <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" s="49" customFormat="1">
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="72"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="98"/>
       <c r="F11" s="54"/>
       <c r="G11" s="51"/>
       <c r="H11" s="51"/>
@@ -2709,9 +2702,9 @@
       <c r="O11" s="51"/>
     </row>
     <row r="12" spans="1:15" s="49" customFormat="1">
-      <c r="B12" s="70"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="72"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="101"/>
       <c r="F12" s="54"/>
       <c r="G12" s="51"/>
       <c r="H12" s="51"/>
@@ -2723,32 +2716,14 @@
       <c r="N12" s="51"/>
       <c r="O12" s="51"/>
     </row>
-    <row r="13" spans="1:15" s="49" customFormat="1">
-      <c r="B13" s="73"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="75"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="F14" s="38"/>
+    <row r="13" spans="1:15">
+      <c r="F13" s="38"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <protectedRanges>
-    <protectedRange sqref="A2:XFD4" name="範囲1"/>
-  </protectedRanges>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
-    <mergeCell ref="B9:D13"/>
     <mergeCell ref="G5:N5"/>
+    <mergeCell ref="B9:D12"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2759,7 +2734,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2812,10 +2787,10 @@
         <v>4</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M1" s="3"/>
     </row>
@@ -3069,19 +3044,19 @@
         <v>60</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D18" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>67</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>69</v>
       </c>
       <c r="H18" s="31" t="s">
         <v>61</v>
@@ -3090,13 +3065,13 @@
         <v>38</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M18" s="33"/>
     </row>
@@ -3109,53 +3084,47 @@
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B21" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="78"/>
+      <c r="B21" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="87"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="81"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="90"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="B23" s="79"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="81"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="90"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="B24" s="79"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="81"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="90"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="B25" s="79"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="81"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="90"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="B26" s="79"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="81"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="B27" s="82"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="84"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="93"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="B21:E27"/>
+    <mergeCell ref="B21:E26"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update explanation of identifier column
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/structure-books.xlsx
+++ b/chiloPro/template-series/structure-books.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chilo-producer\chiloPro\template-series\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -390,12 +390,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>CHiLO BookのユニークID。
-──────────────────
-content.opfに設定されます。</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>各CHiLO Bookの概要
 ────────────
 「はじめにお読みください」セクションの「ブック概要」に挿入されます。</t>
@@ -935,6 +929,12 @@
 ・ page-typeを指定して、行を追加するとCHiLO Bookのページが追加されます。
 ・ ブックの数だけ書籍構成シートをコピーして、1冊のブックにつき1シート作成します。
 ・ シート名は、book-listの「vol」の列と一致させてください。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CHiLO BookのUUID。
+──────────────────
+content.opfに設定されます。</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1856,11 +1856,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1897,30 +1921,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -2285,7 +2285,7 @@
         <v>55</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1">
@@ -2297,19 +2297,19 @@
         <v>45</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1">
       <c r="A3" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="25" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="72"/>
     </row>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="72"/>
     </row>
@@ -2402,10 +2402,10 @@
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1">
       <c r="A12" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>35</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" s="75"/>
       <c r="C15" s="76"/>
@@ -2486,7 +2486,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E1" s="45" t="s">
         <v>40</v>
@@ -2495,31 +2495,31 @@
         <v>13</v>
       </c>
       <c r="G1" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="47" t="s">
+      <c r="N1" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="N1" s="47" t="s">
+      <c r="O1" s="47" t="s">
         <v>77</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="48" customHeight="1" thickTop="1">
@@ -2580,32 +2580,32 @@
         <v>56</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="48" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="55" t="s">
         <v>79</v>
-      </c>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="55" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="49" customFormat="1">
@@ -2654,11 +2654,11 @@
     </row>
     <row r="9" spans="1:15" s="49" customFormat="1" ht="14.25" customHeight="1">
       <c r="A9" s="53"/>
-      <c r="B9" s="83" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="95"/>
+      <c r="B9" s="84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="85"/>
+      <c r="D9" s="86"/>
       <c r="F9" s="54"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
@@ -2672,9 +2672,9 @@
     </row>
     <row r="10" spans="1:15" s="49" customFormat="1">
       <c r="A10" s="53"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="F10" s="54"/>
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
@@ -2687,9 +2687,9 @@
       <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" s="49" customFormat="1">
-      <c r="B11" s="96"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="98"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89"/>
       <c r="F11" s="54"/>
       <c r="G11" s="51"/>
       <c r="H11" s="51"/>
@@ -2702,9 +2702,9 @@
       <c r="O11" s="51"/>
     </row>
     <row r="12" spans="1:15" s="49" customFormat="1">
-      <c r="B12" s="99"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="101"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="92"/>
       <c r="F12" s="54"/>
       <c r="G12" s="51"/>
       <c r="H12" s="51"/>
@@ -2787,10 +2787,10 @@
         <v>4</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="M1" s="3"/>
     </row>
@@ -3038,40 +3038,40 @@
     </row>
     <row r="18" spans="1:13" s="34" customFormat="1" ht="165" customHeight="1">
       <c r="A18" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="31" t="s">
         <v>60</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>61</v>
       </c>
       <c r="I18" s="31" t="s">
         <v>38</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K18" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="L18" s="31" t="s">
         <v>83</v>
-      </c>
-      <c r="L18" s="31" t="s">
-        <v>84</v>
       </c>
       <c r="M18" s="33"/>
     </row>
@@ -3084,42 +3084,42 @@
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B21" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="87"/>
+      <c r="B21" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="90"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="98"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="B23" s="88"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="90"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="98"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="90"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="98"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="B25" s="88"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="90"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="98"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="B26" s="91"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="93"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="101"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>